<commit_message>
Location Multiple upload validation
</commit_message>
<xml_diff>
--- a/src/assets/files/DepartmentUpload.xlsx
+++ b/src/assets/files/DepartmentUpload.xlsx
@@ -33,9 +33,6 @@
     <t>Department Head</t>
   </si>
   <si>
-    <t xml:space="preserve">D001 </t>
-  </si>
-  <si>
     <t>HR Department</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>sample@gmail.com</t>
+  </si>
+  <si>
+    <t>D001</t>
   </si>
 </sst>
 </file>
@@ -96,14 +96,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDCE6F2"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <fgColor theme="4"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor rgb="FF808080"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -169,16 +169,16 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -578,7 +578,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -605,53 +605,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="10"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>